<commit_message>
Changes to Fluke Command sheet
Testing data collection
</commit_message>
<xml_diff>
--- a/raw.simulated2.xlsx
+++ b/raw.simulated2.xlsx
@@ -9,6 +9,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Results" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Results1" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Results2" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -56560,4 +56561,4343 @@
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F216"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C1" t="s">
+        <v>308</v>
+      </c>
+      <c r="D1" t="s">
+        <v>309</v>
+      </c>
+      <c r="E1" t="s">
+        <v>310</v>
+      </c>
+      <c r="F1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1.000650360751949</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.001595446567756859</v>
+      </c>
+      <c r="D2" t="n">
+        <v>72.08846289032512</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>313</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1.000650360751949</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.001663622860775236</v>
+      </c>
+      <c r="D3" t="n">
+        <v>43.97536668558032</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.987362363395239</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.001417275802951085</v>
+      </c>
+      <c r="D4" t="n">
+        <v>70.42308859719853</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>313</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.987362363395239</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.001130549719282247</v>
+      </c>
+      <c r="D5" t="n">
+        <v>211.0022302065207</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>314</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1.004069746528306</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.001727434775194335</v>
+      </c>
+      <c r="D6" t="n">
+        <v>60.38070476130275</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>315</v>
+      </c>
+      <c r="B7" t="n">
+        <v>-0.9989069099460364</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.001048769220182512</v>
+      </c>
+      <c r="D7" t="n">
+        <v>254.0494354604196</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>314</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1.015338870442298</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.001959487349302241</v>
+      </c>
+      <c r="D8" t="n">
+        <v>58.01020443812631</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>315</v>
+      </c>
+      <c r="B9" t="n">
+        <v>-1.019749252472122</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.001356049993155858</v>
+      </c>
+      <c r="D9" t="n">
+        <v>116.5256304327307</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>306</v>
+      </c>
+      <c r="B10" t="s">
+        <v>307</v>
+      </c>
+      <c r="C10" t="s">
+        <v>308</v>
+      </c>
+      <c r="D10" t="s">
+        <v>309</v>
+      </c>
+      <c r="E10" t="s">
+        <v>310</v>
+      </c>
+      <c r="F10" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>312</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1.004554401177696</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.001931803115054581</v>
+      </c>
+      <c r="D11" t="n">
+        <v>65.40203907502845</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-0.001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>313</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1.004554401177696</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.001510650303184627</v>
+      </c>
+      <c r="D12" t="n">
+        <v>69.7349058069379</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-0.001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>312</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.9954841192526372</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.001251271325072699</v>
+      </c>
+      <c r="D13" t="n">
+        <v>95.15984490534531</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F13" t="n">
+        <v>-0.001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>313</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.9954841192526372</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.001181931863377983</v>
+      </c>
+      <c r="D14" t="n">
+        <v>150.075188002736</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-0.001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>314</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0.9927716465321567</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.001823855165578219</v>
+      </c>
+      <c r="D15" t="n">
+        <v>70.98072549719986</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F15" t="n">
+        <v>-0.001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>315</v>
+      </c>
+      <c r="B16" t="n">
+        <v>-0.9931845626457979</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.001153247886288611</v>
+      </c>
+      <c r="D16" t="n">
+        <v>308.9851201418962</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F16" t="n">
+        <v>-0.001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>314</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0.9992026147711749</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.001520849325957005</v>
+      </c>
+      <c r="D17" t="n">
+        <v>86.89141597312199</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F17" t="n">
+        <v>-0.001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>315</v>
+      </c>
+      <c r="B18" t="n">
+        <v>-0.01007934570681294</v>
+      </c>
+      <c r="C18" t="n">
+        <v>9.293778818405846e-06</v>
+      </c>
+      <c r="D18" t="n">
+        <v>270.0584129383068</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F18" t="n">
+        <v>-0.001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>306</v>
+      </c>
+      <c r="B19" t="s">
+        <v>307</v>
+      </c>
+      <c r="C19" t="s">
+        <v>308</v>
+      </c>
+      <c r="D19" t="s">
+        <v>309</v>
+      </c>
+      <c r="E19" t="s">
+        <v>310</v>
+      </c>
+      <c r="F19" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>312</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0.9983698448938131</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.0002110933322817651</v>
+      </c>
+      <c r="D20" t="n">
+        <v>47.7760139001487</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>313</v>
+      </c>
+      <c r="B21" t="n">
+        <v>0.9983698448938131</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.0001534309380148454</v>
+      </c>
+      <c r="D21" t="n">
+        <v>46.38045072078077</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>312</v>
+      </c>
+      <c r="B22" t="n">
+        <v>0.9996137481483651</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.0001363394092587745</v>
+      </c>
+      <c r="D22" t="n">
+        <v>56.57735339550472</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>313</v>
+      </c>
+      <c r="B23" t="n">
+        <v>0.9996137481483651</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.0001007519086147505</v>
+      </c>
+      <c r="D23" t="n">
+        <v>174.4635912252799</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>314</v>
+      </c>
+      <c r="B24" t="n">
+        <v>0.9977661870824004</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.0001858651996674105</v>
+      </c>
+      <c r="D24" t="n">
+        <v>38.72915878513699</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>315</v>
+      </c>
+      <c r="B25" t="n">
+        <v>-0.9994662275631596</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.0001131630033818712</v>
+      </c>
+      <c r="D25" t="n">
+        <v>182.1180492480357</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>314</v>
+      </c>
+      <c r="B26" t="n">
+        <v>0.9960244827676762</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.0001772749741572739</v>
+      </c>
+      <c r="D26" t="n">
+        <v>65.4050688438509</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>315</v>
+      </c>
+      <c r="B27" t="n">
+        <v>-0.09930115058373451</v>
+      </c>
+      <c r="C27" t="n">
+        <v>9.059882767188991e-06</v>
+      </c>
+      <c r="D27" t="n">
+        <v>236.3030558735081</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>306</v>
+      </c>
+      <c r="B28" t="s">
+        <v>307</v>
+      </c>
+      <c r="C28" t="s">
+        <v>308</v>
+      </c>
+      <c r="D28" t="s">
+        <v>309</v>
+      </c>
+      <c r="E28" t="s">
+        <v>310</v>
+      </c>
+      <c r="F28" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>312</v>
+      </c>
+      <c r="B29" t="n">
+        <v>1.014676775053536</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.0001978190637763657</v>
+      </c>
+      <c r="D29" t="n">
+        <v>57.06783370306029</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F29" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>313</v>
+      </c>
+      <c r="B30" t="n">
+        <v>1.014676775053536</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.0001570945381877632</v>
+      </c>
+      <c r="D30" t="n">
+        <v>52.45477507797388</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F30" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>312</v>
+      </c>
+      <c r="B31" t="n">
+        <v>1.00034852618124</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.0001388745922276529</v>
+      </c>
+      <c r="D31" t="n">
+        <v>108.2165396717758</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F31" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>313</v>
+      </c>
+      <c r="B32" t="n">
+        <v>1.00034852618124</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.0001235617417062838</v>
+      </c>
+      <c r="D32" t="n">
+        <v>167.6491725958214</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F32" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>314</v>
+      </c>
+      <c r="B33" t="n">
+        <v>0.9831171293924675</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0.0001857064613669412</v>
+      </c>
+      <c r="D33" t="n">
+        <v>59.96907633786596</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F33" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>315</v>
+      </c>
+      <c r="B34" t="n">
+        <v>-0.09879789818007431</v>
+      </c>
+      <c r="C34" t="n">
+        <v>9.431930246465604e-06</v>
+      </c>
+      <c r="D34" t="n">
+        <v>285.9222393491638</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F34" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>314</v>
+      </c>
+      <c r="B35" t="n">
+        <v>1.003711186485095</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0.0001857277750355647</v>
+      </c>
+      <c r="D35" t="n">
+        <v>58.1059872471165</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F35" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>315</v>
+      </c>
+      <c r="B36" t="n">
+        <v>-0.9963301358398463</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0.0001793895805889256</v>
+      </c>
+      <c r="D36" t="n">
+        <v>51.09120368412852</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F36" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>306</v>
+      </c>
+      <c r="B37" t="s">
+        <v>307</v>
+      </c>
+      <c r="C37" t="s">
+        <v>308</v>
+      </c>
+      <c r="D37" t="s">
+        <v>309</v>
+      </c>
+      <c r="E37" t="s">
+        <v>310</v>
+      </c>
+      <c r="F37" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
+        <v>312</v>
+      </c>
+      <c r="B38" t="n">
+        <v>1.001389986948592</v>
+      </c>
+      <c r="C38" t="n">
+        <v>1.665136414980998e-05</v>
+      </c>
+      <c r="D38" t="n">
+        <v>110.4978211991045</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>313</v>
+      </c>
+      <c r="B39" t="n">
+        <v>1.001389986948592</v>
+      </c>
+      <c r="C39" t="n">
+        <v>2.3667223081601e-05</v>
+      </c>
+      <c r="D39" t="n">
+        <v>44.36625964426096</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>312</v>
+      </c>
+      <c r="B40" t="n">
+        <v>0.9928999187686308</v>
+      </c>
+      <c r="C40" t="n">
+        <v>3.27032172825802e-05</v>
+      </c>
+      <c r="D40" t="n">
+        <v>44.47324493346638</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>313</v>
+      </c>
+      <c r="B41" t="n">
+        <v>0.9928999187686308</v>
+      </c>
+      <c r="C41" t="n">
+        <v>3.05859364857457e-05</v>
+      </c>
+      <c r="D41" t="n">
+        <v>43.99117161652802</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
+        <v>314</v>
+      </c>
+      <c r="B42" t="n">
+        <v>1.001772476374085</v>
+      </c>
+      <c r="C42" t="n">
+        <v>1.887847741513505e-05</v>
+      </c>
+      <c r="D42" t="n">
+        <v>79.23303826303932</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>315</v>
+      </c>
+      <c r="B43" t="n">
+        <v>-0.9999083528838391</v>
+      </c>
+      <c r="C43" t="n">
+        <v>1.554422258510158e-05</v>
+      </c>
+      <c r="D43" t="n">
+        <v>157.1811647407427</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
+        <v>314</v>
+      </c>
+      <c r="B44" t="n">
+        <v>1.001518833312005</v>
+      </c>
+      <c r="C44" t="n">
+        <v>3.356578475642754e-05</v>
+      </c>
+      <c r="D44" t="n">
+        <v>44.23135786281819</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" t="s">
+        <v>315</v>
+      </c>
+      <c r="B45" t="n">
+        <v>-0.1008123359563221</v>
+      </c>
+      <c r="C45" t="n">
+        <v>1.304608470395263e-06</v>
+      </c>
+      <c r="D45" t="n">
+        <v>149.7658861749932</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" t="s">
+        <v>306</v>
+      </c>
+      <c r="B46" t="s">
+        <v>307</v>
+      </c>
+      <c r="C46" t="s">
+        <v>308</v>
+      </c>
+      <c r="D46" t="s">
+        <v>309</v>
+      </c>
+      <c r="E46" t="s">
+        <v>310</v>
+      </c>
+      <c r="F46" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" t="s">
+        <v>312</v>
+      </c>
+      <c r="B47" t="n">
+        <v>1.000090158304167</v>
+      </c>
+      <c r="C47" t="n">
+        <v>2.204302279760055e-05</v>
+      </c>
+      <c r="D47" t="n">
+        <v>57.89089629175054</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F47" t="n">
+        <v>-0.05</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" t="s">
+        <v>313</v>
+      </c>
+      <c r="B48" t="n">
+        <v>1.000090158304167</v>
+      </c>
+      <c r="C48" t="n">
+        <v>2.24918627824139e-05</v>
+      </c>
+      <c r="D48" t="n">
+        <v>71.12428567093744</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F48" t="n">
+        <v>-0.05</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" t="s">
+        <v>312</v>
+      </c>
+      <c r="B49" t="n">
+        <v>1.001282539397067</v>
+      </c>
+      <c r="C49" t="n">
+        <v>6.61687079676554e-06</v>
+      </c>
+      <c r="D49" t="n">
+        <v>69.88335087142201</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F49" t="n">
+        <v>-0.05</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" t="s">
+        <v>313</v>
+      </c>
+      <c r="B50" t="n">
+        <v>1.001282539397067</v>
+      </c>
+      <c r="C50" t="n">
+        <v>1.155354886750939e-05</v>
+      </c>
+      <c r="D50" t="n">
+        <v>45.50465707597712</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F50" t="n">
+        <v>-0.05</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" t="s">
+        <v>314</v>
+      </c>
+      <c r="B51" t="n">
+        <v>1.002504954779342</v>
+      </c>
+      <c r="C51" t="n">
+        <v>2.74003174635934e-05</v>
+      </c>
+      <c r="D51" t="n">
+        <v>47.78580659857785</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F51" t="n">
+        <v>-0.05</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" t="s">
+        <v>315</v>
+      </c>
+      <c r="B52" t="n">
+        <v>-0.1002895189973403</v>
+      </c>
+      <c r="C52" t="n">
+        <v>1.216996995655719e-06</v>
+      </c>
+      <c r="D52" t="n">
+        <v>170.9135721109064</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F52" t="n">
+        <v>-0.05</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" t="s">
+        <v>314</v>
+      </c>
+      <c r="B53" t="n">
+        <v>0.9985379985242193</v>
+      </c>
+      <c r="C53" t="n">
+        <v>6.048060242491301e-06</v>
+      </c>
+      <c r="D53" t="n">
+        <v>119.6946470321864</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F53" t="n">
+        <v>-0.05</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" t="s">
+        <v>315</v>
+      </c>
+      <c r="B54" t="n">
+        <v>-0.9993961692443202</v>
+      </c>
+      <c r="C54" t="n">
+        <v>9.698314469175083e-06</v>
+      </c>
+      <c r="D54" t="n">
+        <v>64.62387492068922</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F54" t="n">
+        <v>-0.05</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" t="s">
+        <v>306</v>
+      </c>
+      <c r="B55" t="s">
+        <v>307</v>
+      </c>
+      <c r="C55" t="s">
+        <v>308</v>
+      </c>
+      <c r="D55" t="s">
+        <v>309</v>
+      </c>
+      <c r="E55" t="s">
+        <v>310</v>
+      </c>
+      <c r="F55" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" t="s">
+        <v>312</v>
+      </c>
+      <c r="B56" t="n">
+        <v>1.00097250874787</v>
+      </c>
+      <c r="C56" t="n">
+        <v>7.797331887466013e-06</v>
+      </c>
+      <c r="D56" t="n">
+        <v>30.54099515433096</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F56" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" t="s">
+        <v>313</v>
+      </c>
+      <c r="B57" t="n">
+        <v>1.00097250874787</v>
+      </c>
+      <c r="C57" t="n">
+        <v>7.493877148088963e-06</v>
+      </c>
+      <c r="D57" t="n">
+        <v>38.0491744842829</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" t="s">
+        <v>312</v>
+      </c>
+      <c r="B58" t="n">
+        <v>1.010730344848851</v>
+      </c>
+      <c r="C58" t="n">
+        <v>7.060100485591176e-06</v>
+      </c>
+      <c r="D58" t="n">
+        <v>44.56549033400589</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" t="s">
+        <v>313</v>
+      </c>
+      <c r="B59" t="n">
+        <v>1.010730344848851</v>
+      </c>
+      <c r="C59" t="n">
+        <v>7.813947337643299e-06</v>
+      </c>
+      <c r="D59" t="n">
+        <v>44.09012561486629</v>
+      </c>
+      <c r="E59" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F59" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" t="s">
+        <v>314</v>
+      </c>
+      <c r="B60" t="n">
+        <v>0.9894949309384271</v>
+      </c>
+      <c r="C60" t="n">
+        <v>5.097971514200595e-06</v>
+      </c>
+      <c r="D60" t="n">
+        <v>51.16672457061457</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F60" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" t="s">
+        <v>315</v>
+      </c>
+      <c r="B61" t="n">
+        <v>-0.9958338797626521</v>
+      </c>
+      <c r="C61" t="n">
+        <v>5.853577159082381e-06</v>
+      </c>
+      <c r="D61" t="n">
+        <v>48.99843939844389</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F61" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" t="s">
+        <v>314</v>
+      </c>
+      <c r="B62" t="n">
+        <v>0.9832341696892734</v>
+      </c>
+      <c r="C62" t="n">
+        <v>6.820128564698709e-06</v>
+      </c>
+      <c r="D62" t="n">
+        <v>45.00224631303268</v>
+      </c>
+      <c r="E62" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" t="s">
+        <v>315</v>
+      </c>
+      <c r="B63" t="n">
+        <v>-0.9804597658423007</v>
+      </c>
+      <c r="C63" t="n">
+        <v>7.527538454892353e-06</v>
+      </c>
+      <c r="D63" t="n">
+        <v>44.49048087707953</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F63" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" t="s">
+        <v>306</v>
+      </c>
+      <c r="B64" t="s">
+        <v>307</v>
+      </c>
+      <c r="C64" t="s">
+        <v>308</v>
+      </c>
+      <c r="D64" t="s">
+        <v>309</v>
+      </c>
+      <c r="E64" t="s">
+        <v>310</v>
+      </c>
+      <c r="F64" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" t="s">
+        <v>312</v>
+      </c>
+      <c r="B65" t="n">
+        <v>0.9891824706860606</v>
+      </c>
+      <c r="C65" t="n">
+        <v>6.989145009338303e-06</v>
+      </c>
+      <c r="D65" t="n">
+        <v>47.07576865084685</v>
+      </c>
+      <c r="E65" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F65" t="n">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" t="s">
+        <v>313</v>
+      </c>
+      <c r="B66" t="n">
+        <v>0.9891824706860606</v>
+      </c>
+      <c r="C66" t="n">
+        <v>7.734459006360811e-06</v>
+      </c>
+      <c r="D66" t="n">
+        <v>46.11586415167665</v>
+      </c>
+      <c r="E66" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F66" t="n">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" t="s">
+        <v>312</v>
+      </c>
+      <c r="B67" t="n">
+        <v>0.9981225144038739</v>
+      </c>
+      <c r="C67" t="n">
+        <v>7.052266108502831e-06</v>
+      </c>
+      <c r="D67" t="n">
+        <v>46.88800002634123</v>
+      </c>
+      <c r="E67" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F67" t="n">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" t="s">
+        <v>313</v>
+      </c>
+      <c r="B68" t="n">
+        <v>0.9981225144038739</v>
+      </c>
+      <c r="C68" t="n">
+        <v>7.79790636770274e-06</v>
+      </c>
+      <c r="D68" t="n">
+        <v>45.96517357928056</v>
+      </c>
+      <c r="E68" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F68" t="n">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" t="s">
+        <v>314</v>
+      </c>
+      <c r="B69" t="n">
+        <v>1.010633888678855</v>
+      </c>
+      <c r="C69" t="n">
+        <v>7.107625521602484e-06</v>
+      </c>
+      <c r="D69" t="n">
+        <v>46.63494510372674</v>
+      </c>
+      <c r="E69" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F69" t="n">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" t="s">
+        <v>315</v>
+      </c>
+      <c r="B70" t="n">
+        <v>-1.01388765729887</v>
+      </c>
+      <c r="C70" t="n">
+        <v>7.898618879314823e-06</v>
+      </c>
+      <c r="D70" t="n">
+        <v>45.70957257988788</v>
+      </c>
+      <c r="E70" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F70" t="n">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" t="s">
+        <v>314</v>
+      </c>
+      <c r="B71" t="n">
+        <v>1.002909228429572</v>
+      </c>
+      <c r="C71" t="n">
+        <v>7.061525076996863e-06</v>
+      </c>
+      <c r="D71" t="n">
+        <v>46.78987329633598</v>
+      </c>
+      <c r="E71" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F71" t="n">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" t="s">
+        <v>315</v>
+      </c>
+      <c r="B72" t="n">
+        <v>-0.9997926914389029</v>
+      </c>
+      <c r="C72" t="n">
+        <v>7.758508460401842e-06</v>
+      </c>
+      <c r="D72" t="n">
+        <v>45.93749173823397</v>
+      </c>
+      <c r="E72" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F72" t="n">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" t="s">
+        <v>306</v>
+      </c>
+      <c r="B73" t="s">
+        <v>307</v>
+      </c>
+      <c r="C73" t="s">
+        <v>308</v>
+      </c>
+      <c r="D73" t="s">
+        <v>309</v>
+      </c>
+      <c r="E73" t="s">
+        <v>310</v>
+      </c>
+      <c r="F73" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" t="s">
+        <v>312</v>
+      </c>
+      <c r="B74" t="n">
+        <v>1.01131415310902</v>
+      </c>
+      <c r="C74" t="n">
+        <v>1.429104065738436e-06</v>
+      </c>
+      <c r="D74" t="n">
+        <v>46.62150004137656</v>
+      </c>
+      <c r="E74" t="n">
+        <v>1</v>
+      </c>
+      <c r="F74" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75" t="s">
+        <v>313</v>
+      </c>
+      <c r="B75" t="n">
+        <v>0.5040285762840233</v>
+      </c>
+      <c r="C75" t="n">
+        <v>4.417246988456269e-07</v>
+      </c>
+      <c r="D75" t="n">
+        <v>72.6778060595709</v>
+      </c>
+      <c r="E75" t="n">
+        <v>1</v>
+      </c>
+      <c r="F75" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" t="s">
+        <v>312</v>
+      </c>
+      <c r="B76" t="n">
+        <v>0.9946677326223849</v>
+      </c>
+      <c r="C76" t="n">
+        <v>1.405573215608901e-06</v>
+      </c>
+      <c r="D76" t="n">
+        <v>46.95985726608114</v>
+      </c>
+      <c r="E76" t="n">
+        <v>1</v>
+      </c>
+      <c r="F76" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" t="s">
+        <v>313</v>
+      </c>
+      <c r="B77" t="n">
+        <v>0.9946677326223849</v>
+      </c>
+      <c r="C77" t="n">
+        <v>1.554676322604335e-06</v>
+      </c>
+      <c r="D77" t="n">
+        <v>46.02289988130276</v>
+      </c>
+      <c r="E77" t="n">
+        <v>1</v>
+      </c>
+      <c r="F77" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" t="s">
+        <v>314</v>
+      </c>
+      <c r="B78" t="n">
+        <v>0.9859323511512557</v>
+      </c>
+      <c r="C78" t="n">
+        <v>1.383120456740616e-06</v>
+      </c>
+      <c r="D78" t="n">
+        <v>47.14552346225364</v>
+      </c>
+      <c r="E78" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F78" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" t="s">
+        <v>315</v>
+      </c>
+      <c r="B79" t="n">
+        <v>-0.4919501022913682</v>
+      </c>
+      <c r="C79" t="n">
+        <v>4.315023587464606e-07</v>
+      </c>
+      <c r="D79" t="n">
+        <v>74.61690171225106</v>
+      </c>
+      <c r="E79" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F79" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" t="s">
+        <v>314</v>
+      </c>
+      <c r="B80" t="n">
+        <v>1.004203047078512</v>
+      </c>
+      <c r="C80" t="n">
+        <v>1.411189560005928e-06</v>
+      </c>
+      <c r="D80" t="n">
+        <v>46.76363193688668</v>
+      </c>
+      <c r="E80" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F80" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" t="s">
+        <v>315</v>
+      </c>
+      <c r="B81" t="n">
+        <v>-1.001950659980248</v>
+      </c>
+      <c r="C81" t="n">
+        <v>1.552861842089304e-06</v>
+      </c>
+      <c r="D81" t="n">
+        <v>45.90194037492302</v>
+      </c>
+      <c r="E81" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F81" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" t="s">
+        <v>306</v>
+      </c>
+      <c r="B82" t="s">
+        <v>307</v>
+      </c>
+      <c r="C82" t="s">
+        <v>308</v>
+      </c>
+      <c r="D82" t="s">
+        <v>309</v>
+      </c>
+      <c r="E82" t="s">
+        <v>310</v>
+      </c>
+      <c r="F82" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" t="s">
+        <v>312</v>
+      </c>
+      <c r="B83" t="n">
+        <v>1.007269043533906</v>
+      </c>
+      <c r="C83" t="n">
+        <v>1.423382078154564e-05</v>
+      </c>
+      <c r="D83" t="n">
+        <v>46.70191887706681</v>
+      </c>
+      <c r="E83" t="n">
+        <v>1</v>
+      </c>
+      <c r="F83" t="n">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" t="s">
+        <v>313</v>
+      </c>
+      <c r="B84" t="n">
+        <v>1.007269043533906</v>
+      </c>
+      <c r="C84" t="n">
+        <v>1.57257456356991e-05</v>
+      </c>
+      <c r="D84" t="n">
+        <v>45.8153455843857</v>
+      </c>
+      <c r="E84" t="n">
+        <v>1</v>
+      </c>
+      <c r="F84" t="n">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" t="s">
+        <v>312</v>
+      </c>
+      <c r="B85" t="n">
+        <v>1.00200836679552</v>
+      </c>
+      <c r="C85" t="n">
+        <v>1.415944381921183e-05</v>
+      </c>
+      <c r="D85" t="n">
+        <v>46.80821501966339</v>
+      </c>
+      <c r="E85" t="n">
+        <v>1</v>
+      </c>
+      <c r="F85" t="n">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" t="s">
+        <v>313</v>
+      </c>
+      <c r="B86" t="n">
+        <v>1.00200836679552</v>
+      </c>
+      <c r="C86" t="n">
+        <v>1.565100090213343e-05</v>
+      </c>
+      <c r="D86" t="n">
+        <v>45.90099299936779</v>
+      </c>
+      <c r="E86" t="n">
+        <v>1</v>
+      </c>
+      <c r="F86" t="n">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" t="s">
+        <v>314</v>
+      </c>
+      <c r="B87" t="n">
+        <v>0.9993268537908425</v>
+      </c>
+      <c r="C87" t="n">
+        <v>1.409365455264339e-05</v>
+      </c>
+      <c r="D87" t="n">
+        <v>46.86315563577261</v>
+      </c>
+      <c r="E87" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F87" t="n">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" t="s">
+        <v>315</v>
+      </c>
+      <c r="B88" t="n">
+        <v>-0.9938623422729782</v>
+      </c>
+      <c r="C88" t="n">
+        <v>1.541986206302045e-05</v>
+      </c>
+      <c r="D88" t="n">
+        <v>46.0364483113258</v>
+      </c>
+      <c r="E88" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F88" t="n">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" t="s">
+        <v>314</v>
+      </c>
+      <c r="B89" t="n">
+        <v>0.9973188433731388</v>
+      </c>
+      <c r="C89" t="n">
+        <v>1.396371532632123e-05</v>
+      </c>
+      <c r="D89" t="n">
+        <v>46.90463774362128</v>
+      </c>
+      <c r="E89" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F89" t="n">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" t="s">
+        <v>315</v>
+      </c>
+      <c r="B90" t="n">
+        <v>-1.006244388321953</v>
+      </c>
+      <c r="C90" t="n">
+        <v>1.570617417448022e-05</v>
+      </c>
+      <c r="D90" t="n">
+        <v>45.83191705161454</v>
+      </c>
+      <c r="E90" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F90" t="n">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91" t="s">
+        <v>306</v>
+      </c>
+      <c r="B91" t="s">
+        <v>307</v>
+      </c>
+      <c r="C91" t="s">
+        <v>308</v>
+      </c>
+      <c r="D91" t="s">
+        <v>309</v>
+      </c>
+      <c r="E91" t="s">
+        <v>310</v>
+      </c>
+      <c r="F91" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92" t="s">
+        <v>312</v>
+      </c>
+      <c r="B92" t="n">
+        <v>1.006583756564875</v>
+      </c>
+      <c r="C92" t="n">
+        <v>7.112064787092174e-07</v>
+      </c>
+      <c r="D92" t="n">
+        <v>46.71565523415135</v>
+      </c>
+      <c r="E92" t="n">
+        <v>1</v>
+      </c>
+      <c r="F92" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93" t="s">
+        <v>313</v>
+      </c>
+      <c r="B93" t="n">
+        <v>1.006583756564875</v>
+      </c>
+      <c r="C93" t="n">
+        <v>7.858003473976797e-07</v>
+      </c>
+      <c r="D93" t="n">
+        <v>45.82642265315354</v>
+      </c>
+      <c r="E93" t="n">
+        <v>1</v>
+      </c>
+      <c r="F93" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94" t="s">
+        <v>312</v>
+      </c>
+      <c r="B94" t="n">
+        <v>1.007190941968878</v>
+      </c>
+      <c r="C94" t="n">
+        <v>7.116358123270914e-07</v>
+      </c>
+      <c r="D94" t="n">
+        <v>46.70348274145065</v>
+      </c>
+      <c r="E94" t="n">
+        <v>1</v>
+      </c>
+      <c r="F94" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95" t="s">
+        <v>313</v>
+      </c>
+      <c r="B95" t="n">
+        <v>1.007190941968878</v>
+      </c>
+      <c r="C95" t="n">
+        <v>7.86231784790895e-07</v>
+      </c>
+      <c r="D95" t="n">
+        <v>45.81660682911032</v>
+      </c>
+      <c r="E95" t="n">
+        <v>1</v>
+      </c>
+      <c r="F95" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="A96" t="s">
+        <v>314</v>
+      </c>
+      <c r="B96" t="n">
+        <v>0.9861953395982108</v>
+      </c>
+      <c r="C96" t="n">
+        <v>6.90991010774529e-07</v>
+      </c>
+      <c r="D96" t="n">
+        <v>47.13984899033778</v>
+      </c>
+      <c r="E96" t="n">
+        <v>1</v>
+      </c>
+      <c r="F96" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
+      <c r="A97" t="s">
+        <v>315</v>
+      </c>
+      <c r="B97" t="n">
+        <v>-0.9938794814895767</v>
+      </c>
+      <c r="C97" t="n">
+        <v>7.762972750029844e-07</v>
+      </c>
+      <c r="D97" t="n">
+        <v>46.03615963136273</v>
+      </c>
+      <c r="E97" t="n">
+        <v>1</v>
+      </c>
+      <c r="F97" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98" t="s">
+        <v>314</v>
+      </c>
+      <c r="B98" t="n">
+        <v>0.989992627812701</v>
+      </c>
+      <c r="C98" t="n">
+        <v>6.96744264758975e-07</v>
+      </c>
+      <c r="D98" t="n">
+        <v>47.05850637148552</v>
+      </c>
+      <c r="E98" t="n">
+        <v>1</v>
+      </c>
+      <c r="F98" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
+      <c r="A99" t="s">
+        <v>315</v>
+      </c>
+      <c r="B99" t="n">
+        <v>-0.98466015186806</v>
+      </c>
+      <c r="C99" t="n">
+        <v>7.630865698069857e-07</v>
+      </c>
+      <c r="D99" t="n">
+        <v>46.19374130960246</v>
+      </c>
+      <c r="E99" t="n">
+        <v>1</v>
+      </c>
+      <c r="F99" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
+      <c r="A100" t="s">
+        <v>306</v>
+      </c>
+      <c r="B100" t="s">
+        <v>307</v>
+      </c>
+      <c r="C100" t="s">
+        <v>308</v>
+      </c>
+      <c r="D100" t="s">
+        <v>309</v>
+      </c>
+      <c r="E100" t="s">
+        <v>310</v>
+      </c>
+      <c r="F100" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6">
+      <c r="A101" t="s">
+        <v>312</v>
+      </c>
+      <c r="B101" t="n">
+        <v>0.9942589965524662</v>
+      </c>
+      <c r="C101" t="n">
+        <v>7.024979932491851e-07</v>
+      </c>
+      <c r="D101" t="n">
+        <v>46.96841689740258</v>
+      </c>
+      <c r="E101" t="n">
+        <v>1</v>
+      </c>
+      <c r="F101" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6">
+      <c r="A102" t="s">
+        <v>313</v>
+      </c>
+      <c r="B102" t="n">
+        <v>0.9942589965524662</v>
+      </c>
+      <c r="C102" t="n">
+        <v>7.770480599118872e-07</v>
+      </c>
+      <c r="D102" t="n">
+        <v>46.02977139003534</v>
+      </c>
+      <c r="E102" t="n">
+        <v>1</v>
+      </c>
+      <c r="F102" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6">
+      <c r="A103" t="s">
+        <v>312</v>
+      </c>
+      <c r="B103" t="n">
+        <v>0.9981097122350141</v>
+      </c>
+      <c r="C103" t="n">
+        <v>7.052175673380283e-07</v>
+      </c>
+      <c r="D103" t="n">
+        <v>46.88826468951329</v>
+      </c>
+      <c r="E103" t="n">
+        <v>1</v>
+      </c>
+      <c r="F103" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6">
+      <c r="A104" t="s">
+        <v>313</v>
+      </c>
+      <c r="B104" t="n">
+        <v>0.9981097122350141</v>
+      </c>
+      <c r="C104" t="n">
+        <v>7.797815473511058e-07</v>
+      </c>
+      <c r="D104" t="n">
+        <v>45.96538632933057</v>
+      </c>
+      <c r="E104" t="n">
+        <v>1</v>
+      </c>
+      <c r="F104" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6">
+      <c r="A105" t="s">
+        <v>314</v>
+      </c>
+      <c r="B105" t="n">
+        <v>0.9980993594731637</v>
+      </c>
+      <c r="C105" t="n">
+        <v>6.992486341663587e-07</v>
+      </c>
+      <c r="D105" t="n">
+        <v>46.8884787240726</v>
+      </c>
+      <c r="E105" t="n">
+        <v>1</v>
+      </c>
+      <c r="F105" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6">
+      <c r="A106" t="s">
+        <v>315</v>
+      </c>
+      <c r="B106" t="n">
+        <v>1.002663004777861</v>
+      </c>
+      <c r="C106" t="n">
+        <v>7.79945595411351e-07</v>
+      </c>
+      <c r="D106" t="n">
+        <v>45.89025781046331</v>
+      </c>
+      <c r="E106" t="n">
+        <v>1</v>
+      </c>
+      <c r="F106" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6">
+      <c r="A107" t="s">
+        <v>314</v>
+      </c>
+      <c r="B107" t="n">
+        <v>0.9958097668781365</v>
+      </c>
+      <c r="C107" t="n">
+        <v>6.987176699702382e-07</v>
+      </c>
+      <c r="D107" t="n">
+        <v>46.93600661052342</v>
+      </c>
+      <c r="E107" t="n">
+        <v>1</v>
+      </c>
+      <c r="F107" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6">
+      <c r="A108" t="s">
+        <v>315</v>
+      </c>
+      <c r="B108" t="n">
+        <v>-0.9997533270835026</v>
+      </c>
+      <c r="C108" t="n">
+        <v>7.786083959374858e-07</v>
+      </c>
+      <c r="D108" t="n">
+        <v>45.93814249303721</v>
+      </c>
+      <c r="E108" t="n">
+        <v>1</v>
+      </c>
+      <c r="F108" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6">
+      <c r="A109" t="s">
+        <v>306</v>
+      </c>
+      <c r="B109" t="s">
+        <v>307</v>
+      </c>
+      <c r="C109" t="s">
+        <v>308</v>
+      </c>
+      <c r="D109" t="s">
+        <v>309</v>
+      </c>
+      <c r="E109" t="s">
+        <v>310</v>
+      </c>
+      <c r="F109" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6">
+      <c r="A110" t="s">
+        <v>312</v>
+      </c>
+      <c r="B110" t="n">
+        <v>0.9977549127315047</v>
+      </c>
+      <c r="C110" t="n">
+        <v>1.409933880903186e-06</v>
+      </c>
+      <c r="D110" t="n">
+        <v>46.89560432177693</v>
+      </c>
+      <c r="E110" t="n">
+        <v>10</v>
+      </c>
+      <c r="F110" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6">
+      <c r="A111" t="s">
+        <v>313</v>
+      </c>
+      <c r="B111" t="n">
+        <v>0.9977549127315047</v>
+      </c>
+      <c r="C111" t="n">
+        <v>1.559059294564471e-06</v>
+      </c>
+      <c r="D111" t="n">
+        <v>45.97128591384057</v>
+      </c>
+      <c r="E111" t="n">
+        <v>10</v>
+      </c>
+      <c r="F111" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6">
+      <c r="A112" t="s">
+        <v>312</v>
+      </c>
+      <c r="B112" t="n">
+        <v>1.006195834920207</v>
+      </c>
+      <c r="C112" t="n">
+        <v>1.421864397512265e-06</v>
+      </c>
+      <c r="D112" t="n">
+        <v>46.72344556298401</v>
+      </c>
+      <c r="E112" t="n">
+        <v>10</v>
+      </c>
+      <c r="F112" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6">
+      <c r="A113" t="s">
+        <v>313</v>
+      </c>
+      <c r="B113" t="n">
+        <v>1.006195834920207</v>
+      </c>
+      <c r="C113" t="n">
+        <v>1.571049441513397e-06</v>
+      </c>
+      <c r="D113" t="n">
+        <v>45.83270361265975</v>
+      </c>
+      <c r="E113" t="n">
+        <v>10</v>
+      </c>
+      <c r="F113" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6">
+      <c r="A114" t="s">
+        <v>314</v>
+      </c>
+      <c r="B114" t="n">
+        <v>0.9981270293847321</v>
+      </c>
+      <c r="C114" t="n">
+        <v>1.397657164947054e-06</v>
+      </c>
+      <c r="D114" t="n">
+        <v>46.88790668960177</v>
+      </c>
+      <c r="E114" t="n">
+        <v>10</v>
+      </c>
+      <c r="F114" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6">
+      <c r="A115" t="s">
+        <v>315</v>
+      </c>
+      <c r="B115" t="n">
+        <v>-0.9994865557713551</v>
+      </c>
+      <c r="C115" t="n">
+        <v>1.549452349099811e-06</v>
+      </c>
+      <c r="D115" t="n">
+        <v>45.94255477330221</v>
+      </c>
+      <c r="E115" t="n">
+        <v>10</v>
+      </c>
+      <c r="F115" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6">
+      <c r="A116" t="s">
+        <v>314</v>
+      </c>
+      <c r="B116" t="n">
+        <v>0.9934842450995328</v>
+      </c>
+      <c r="C116" t="n">
+        <v>1.396389797003089e-06</v>
+      </c>
+      <c r="D116" t="n">
+        <v>46.98467554789838</v>
+      </c>
+      <c r="E116" t="n">
+        <v>10</v>
+      </c>
+      <c r="F116" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6">
+      <c r="A117" t="s">
+        <v>315</v>
+      </c>
+      <c r="B117" t="n">
+        <v>-0.9950054015308721</v>
+      </c>
+      <c r="C117" t="n">
+        <v>1.549202591246195e-06</v>
+      </c>
+      <c r="D117" t="n">
+        <v>46.01722984179813</v>
+      </c>
+      <c r="E117" t="n">
+        <v>10</v>
+      </c>
+      <c r="F117" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6">
+      <c r="A118" t="s">
+        <v>306</v>
+      </c>
+      <c r="B118" t="s">
+        <v>307</v>
+      </c>
+      <c r="C118" t="s">
+        <v>308</v>
+      </c>
+      <c r="D118" t="s">
+        <v>309</v>
+      </c>
+      <c r="E118" t="s">
+        <v>310</v>
+      </c>
+      <c r="F118" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6">
+      <c r="A119" t="s">
+        <v>312</v>
+      </c>
+      <c r="B119" t="n">
+        <v>1.004206052424618</v>
+      </c>
+      <c r="C119" t="n">
+        <v>1.419051011735791e-06</v>
+      </c>
+      <c r="D119" t="n">
+        <v>46.76357112037246</v>
+      </c>
+      <c r="E119" t="n">
+        <v>10</v>
+      </c>
+      <c r="F119" t="n">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6">
+      <c r="A120" t="s">
+        <v>313</v>
+      </c>
+      <c r="B120" t="n">
+        <v>1.004206052424618</v>
+      </c>
+      <c r="C120" t="n">
+        <v>1.568222176063924e-06</v>
+      </c>
+      <c r="D120" t="n">
+        <v>45.86504112499649</v>
+      </c>
+      <c r="E120" t="n">
+        <v>10</v>
+      </c>
+      <c r="F120" t="n">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6">
+      <c r="A121" t="s">
+        <v>312</v>
+      </c>
+      <c r="B121" t="n">
+        <v>0.9964596784180505</v>
+      </c>
+      <c r="C121" t="n">
+        <v>1.408104168369788e-06</v>
+      </c>
+      <c r="D121" t="n">
+        <v>46.92247654034125</v>
+      </c>
+      <c r="E121" t="n">
+        <v>10</v>
+      </c>
+      <c r="F121" t="n">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6">
+      <c r="A122" t="s">
+        <v>313</v>
+      </c>
+      <c r="B122" t="n">
+        <v>0.9964596784180505</v>
+      </c>
+      <c r="C122" t="n">
+        <v>1.55722025610686e-06</v>
+      </c>
+      <c r="D122" t="n">
+        <v>45.99287926891842</v>
+      </c>
+      <c r="E122" t="n">
+        <v>10</v>
+      </c>
+      <c r="F122" t="n">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6">
+      <c r="A123" t="s">
+        <v>314</v>
+      </c>
+      <c r="B123" t="n">
+        <v>0.9948503432090815</v>
+      </c>
+      <c r="C123" t="n">
+        <v>1.401345979421487e-06</v>
+      </c>
+      <c r="D123" t="n">
+        <v>46.95603708789243</v>
+      </c>
+      <c r="E123" t="n">
+        <v>10</v>
+      </c>
+      <c r="F123" t="n">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6">
+      <c r="A124" t="s">
+        <v>315</v>
+      </c>
+      <c r="B124" t="n">
+        <v>-0.9892236327403094</v>
+      </c>
+      <c r="C124" t="n">
+        <v>1.533293463094892e-06</v>
+      </c>
+      <c r="D124" t="n">
+        <v>46.11516047216081</v>
+      </c>
+      <c r="E124" t="n">
+        <v>10</v>
+      </c>
+      <c r="F124" t="n">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6">
+      <c r="A125" t="s">
+        <v>314</v>
+      </c>
+      <c r="B125" t="n">
+        <v>0.9973051165730251</v>
+      </c>
+      <c r="C125" t="n">
+        <v>1.397422298228205e-06</v>
+      </c>
+      <c r="D125" t="n">
+        <v>46.90492232758048</v>
+      </c>
+      <c r="E125" t="n">
+        <v>10</v>
+      </c>
+      <c r="F125" t="n">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6">
+      <c r="A126" t="s">
+        <v>315</v>
+      </c>
+      <c r="B126" t="n">
+        <v>-0.9966724349377923</v>
+      </c>
+      <c r="C126" t="n">
+        <v>1.54341734179675e-06</v>
+      </c>
+      <c r="D126" t="n">
+        <v>45.98932624531505</v>
+      </c>
+      <c r="E126" t="n">
+        <v>10</v>
+      </c>
+      <c r="F126" t="n">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6">
+      <c r="A127" t="s">
+        <v>306</v>
+      </c>
+      <c r="B127" t="s">
+        <v>307</v>
+      </c>
+      <c r="C127" t="s">
+        <v>308</v>
+      </c>
+      <c r="D127" t="s">
+        <v>309</v>
+      </c>
+      <c r="E127" t="s">
+        <v>310</v>
+      </c>
+      <c r="F127" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6">
+      <c r="A128" t="s">
+        <v>312</v>
+      </c>
+      <c r="B128" t="n">
+        <v>0.9992533363555447</v>
+      </c>
+      <c r="C128" t="n">
+        <v>7.060254797851633e-07</v>
+      </c>
+      <c r="D128" t="n">
+        <v>46.86466921467188</v>
+      </c>
+      <c r="E128" t="n">
+        <v>10</v>
+      </c>
+      <c r="F128" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6">
+      <c r="A129" t="s">
+        <v>313</v>
+      </c>
+      <c r="B129" t="n">
+        <v>0.9992533363555447</v>
+      </c>
+      <c r="C129" t="n">
+        <v>7.805935516071493e-07</v>
+      </c>
+      <c r="D129" t="n">
+        <v>45.94641516387277</v>
+      </c>
+      <c r="E129" t="n">
+        <v>10</v>
+      </c>
+      <c r="F129" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6">
+      <c r="A130" t="s">
+        <v>312</v>
+      </c>
+      <c r="B130" t="n">
+        <v>1.008558222809282</v>
+      </c>
+      <c r="C130" t="n">
+        <v>7.126027040748201e-07</v>
+      </c>
+      <c r="D130" t="n">
+        <v>46.6761664122913</v>
+      </c>
+      <c r="E130" t="n">
+        <v>10</v>
+      </c>
+      <c r="F130" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6">
+      <c r="A131" t="s">
+        <v>313</v>
+      </c>
+      <c r="B131" t="n">
+        <v>1.008558222809282</v>
+      </c>
+      <c r="C131" t="n">
+        <v>7.872033956481424e-07</v>
+      </c>
+      <c r="D131" t="n">
+        <v>45.79457136916446</v>
+      </c>
+      <c r="E131" t="n">
+        <v>10</v>
+      </c>
+      <c r="F131" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6">
+      <c r="A132" t="s">
+        <v>314</v>
+      </c>
+      <c r="B132" t="n">
+        <v>1.009357845915858</v>
+      </c>
+      <c r="C132" t="n">
+        <v>7.130692220898181e-07</v>
+      </c>
+      <c r="D132" t="n">
+        <v>46.66025121744066</v>
+      </c>
+      <c r="E132" t="n">
+        <v>10</v>
+      </c>
+      <c r="F132" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6">
+      <c r="A133" t="s">
+        <v>315</v>
+      </c>
+      <c r="B133" t="n">
+        <v>-1.00850665717957</v>
+      </c>
+      <c r="C133" t="n">
+        <v>7.863937401674768e-07</v>
+      </c>
+      <c r="D133" t="n">
+        <v>45.79540070646</v>
+      </c>
+      <c r="E133" t="n">
+        <v>10</v>
+      </c>
+      <c r="F133" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6">
+      <c r="A134" t="s">
+        <v>314</v>
+      </c>
+      <c r="B134" t="n">
+        <v>0.9996901289309911</v>
+      </c>
+      <c r="C134" t="n">
+        <v>7.059788722324746e-07</v>
+      </c>
+      <c r="D134" t="n">
+        <v>46.85568226131353</v>
+      </c>
+      <c r="E134" t="n">
+        <v>10</v>
+      </c>
+      <c r="F134" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6">
+      <c r="A135" t="s">
+        <v>315</v>
+      </c>
+      <c r="B135" t="n">
+        <v>-0.9962436619435913</v>
+      </c>
+      <c r="C135" t="n">
+        <v>7.753828994542398e-07</v>
+      </c>
+      <c r="D135" t="n">
+        <v>45.99648918280781</v>
+      </c>
+      <c r="E135" t="n">
+        <v>10</v>
+      </c>
+      <c r="F135" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6">
+      <c r="A136" t="s">
+        <v>306</v>
+      </c>
+      <c r="B136" t="s">
+        <v>307</v>
+      </c>
+      <c r="C136" t="s">
+        <v>308</v>
+      </c>
+      <c r="D136" t="s">
+        <v>309</v>
+      </c>
+      <c r="E136" t="s">
+        <v>310</v>
+      </c>
+      <c r="F136" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6">
+      <c r="A137" t="s">
+        <v>312</v>
+      </c>
+      <c r="B137" t="n">
+        <v>1.002947344681583</v>
+      </c>
+      <c r="C137" t="n">
+        <v>7.086358105884246e-07</v>
+      </c>
+      <c r="D137" t="n">
+        <v>46.7890985179554</v>
+      </c>
+      <c r="E137" t="n">
+        <v>10</v>
+      </c>
+      <c r="F137" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6">
+      <c r="A138" t="s">
+        <v>313</v>
+      </c>
+      <c r="B138" t="n">
+        <v>1.002947344681583</v>
+      </c>
+      <c r="C138" t="n">
+        <v>7.832169747262987e-07</v>
+      </c>
+      <c r="D138" t="n">
+        <v>45.88560189603324</v>
+      </c>
+      <c r="E138" t="n">
+        <v>10</v>
+      </c>
+      <c r="F138" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6">
+      <c r="A139" t="s">
+        <v>312</v>
+      </c>
+      <c r="B139" t="n">
+        <v>0.9952999689305493</v>
+      </c>
+      <c r="C139" t="n">
+        <v>7.032330654133503e-07</v>
+      </c>
+      <c r="D139" t="n">
+        <v>46.94664151548374</v>
+      </c>
+      <c r="E139" t="n">
+        <v>10</v>
+      </c>
+      <c r="F139" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6">
+      <c r="A140" t="s">
+        <v>313</v>
+      </c>
+      <c r="B140" t="n">
+        <v>0.9952999689305493</v>
+      </c>
+      <c r="C140" t="n">
+        <v>7.777869140648619e-07</v>
+      </c>
+      <c r="D140" t="n">
+        <v>46.01228850595636</v>
+      </c>
+      <c r="E140" t="n">
+        <v>10</v>
+      </c>
+      <c r="F140" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6">
+      <c r="A141" t="s">
+        <v>314</v>
+      </c>
+      <c r="B141" t="n">
+        <v>0.9971906465855898</v>
+      </c>
+      <c r="C141" t="n">
+        <v>7.034185966672066e-07</v>
+      </c>
+      <c r="D141" t="n">
+        <v>46.90729605547851</v>
+      </c>
+      <c r="E141" t="n">
+        <v>10</v>
+      </c>
+      <c r="F141" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6">
+      <c r="A142" t="s">
+        <v>315</v>
+      </c>
+      <c r="B142" t="n">
+        <v>-0.994449432205217</v>
+      </c>
+      <c r="C142" t="n">
+        <v>7.737820082362744e-07</v>
+      </c>
+      <c r="D142" t="n">
+        <v>46.02656875266585</v>
+      </c>
+      <c r="E142" t="n">
+        <v>10</v>
+      </c>
+      <c r="F142" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6">
+      <c r="A143" t="s">
+        <v>314</v>
+      </c>
+      <c r="B143" t="n">
+        <v>1.001739052315263</v>
+      </c>
+      <c r="C143" t="n">
+        <v>7.0445632718972e-07</v>
+      </c>
+      <c r="D143" t="n">
+        <v>46.81370957462938</v>
+      </c>
+      <c r="E143" t="n">
+        <v>10</v>
+      </c>
+      <c r="F143" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6">
+      <c r="A144" t="s">
+        <v>315</v>
+      </c>
+      <c r="B144" t="n">
+        <v>-1.006451128930213</v>
+      </c>
+      <c r="C144" t="n">
+        <v>7.856929571241123e-07</v>
+      </c>
+      <c r="D144" t="n">
+        <v>45.82856920983171</v>
+      </c>
+      <c r="E144" t="n">
+        <v>10</v>
+      </c>
+      <c r="F144" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6">
+      <c r="A145" t="s">
+        <v>306</v>
+      </c>
+      <c r="B145" t="s">
+        <v>307</v>
+      </c>
+      <c r="C145" t="s">
+        <v>308</v>
+      </c>
+      <c r="D145" t="s">
+        <v>309</v>
+      </c>
+      <c r="E145" t="s">
+        <v>310</v>
+      </c>
+      <c r="F145" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6">
+      <c r="A146" t="s">
+        <v>312</v>
+      </c>
+      <c r="B146" t="n">
+        <v>0.9970293663382627</v>
+      </c>
+      <c r="C146" t="n">
+        <v>6.641664367293076e-08</v>
+      </c>
+      <c r="D146" t="n">
+        <v>58.62278763337758</v>
+      </c>
+      <c r="E146" t="n">
+        <v>10</v>
+      </c>
+      <c r="F146" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6">
+      <c r="A147" t="s">
+        <v>313</v>
+      </c>
+      <c r="B147" t="n">
+        <v>0.9970293663382627</v>
+      </c>
+      <c r="C147" t="n">
+        <v>8.138379711637166e-08</v>
+      </c>
+      <c r="D147" t="n">
+        <v>54.3885901148964</v>
+      </c>
+      <c r="E147" t="n">
+        <v>10</v>
+      </c>
+      <c r="F147" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6">
+      <c r="A148" t="s">
+        <v>312</v>
+      </c>
+      <c r="B148" t="n">
+        <v>0.9931962870678788</v>
+      </c>
+      <c r="C148" t="n">
+        <v>6.616161956953598e-08</v>
+      </c>
+      <c r="D148" t="n">
+        <v>58.83366310924539</v>
+      </c>
+      <c r="E148" t="n">
+        <v>10</v>
+      </c>
+      <c r="F148" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6">
+      <c r="A149" t="s">
+        <v>313</v>
+      </c>
+      <c r="B149" t="n">
+        <v>0.9931962870678788</v>
+      </c>
+      <c r="C149" t="n">
+        <v>8.112340699676249e-08</v>
+      </c>
+      <c r="D149" t="n">
+        <v>54.52278530326159</v>
+      </c>
+      <c r="E149" t="n">
+        <v>10</v>
+      </c>
+      <c r="F149" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6">
+      <c r="A150" t="s">
+        <v>314</v>
+      </c>
+      <c r="B150" t="n">
+        <v>1.000619549185579</v>
+      </c>
+      <c r="C150" t="n">
+        <v>6.613950589190506e-08</v>
+      </c>
+      <c r="D150" t="n">
+        <v>58.42814545558701</v>
+      </c>
+      <c r="E150" t="n">
+        <v>10</v>
+      </c>
+      <c r="F150" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6">
+      <c r="A151" t="s">
+        <v>315</v>
+      </c>
+      <c r="B151" t="n">
+        <v>-1.005226494336646</v>
+      </c>
+      <c r="C151" t="n">
+        <v>8.168094530653941e-08</v>
+      </c>
+      <c r="D151" t="n">
+        <v>54.10706117264247</v>
+      </c>
+      <c r="E151" t="n">
+        <v>10</v>
+      </c>
+      <c r="F151" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6">
+      <c r="A152" t="s">
+        <v>314</v>
+      </c>
+      <c r="B152" t="n">
+        <v>1.010449749677301</v>
+      </c>
+      <c r="C152" t="n">
+        <v>6.7190916482781e-08</v>
+      </c>
+      <c r="D152" t="n">
+        <v>57.90899724515101</v>
+      </c>
+      <c r="E152" t="n">
+        <v>10</v>
+      </c>
+      <c r="F152" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6">
+      <c r="A153" t="s">
+        <v>315</v>
+      </c>
+      <c r="B153" t="n">
+        <v>-1.006130959240738</v>
+      </c>
+      <c r="C153" t="n">
+        <v>8.150604148385089e-08</v>
+      </c>
+      <c r="D153" t="n">
+        <v>54.07644426207074</v>
+      </c>
+      <c r="E153" t="n">
+        <v>10</v>
+      </c>
+      <c r="F153" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6">
+      <c r="A154" t="s">
+        <v>306</v>
+      </c>
+      <c r="B154" t="s">
+        <v>307</v>
+      </c>
+      <c r="C154" t="s">
+        <v>308</v>
+      </c>
+      <c r="D154" t="s">
+        <v>309</v>
+      </c>
+      <c r="E154" t="s">
+        <v>310</v>
+      </c>
+      <c r="F154" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6">
+      <c r="A155" t="s">
+        <v>312</v>
+      </c>
+      <c r="B155" t="n">
+        <v>0.7995296090894082</v>
+      </c>
+      <c r="C155" t="n">
+        <v>5.367714626562653e-08</v>
+      </c>
+      <c r="D155" t="n">
+        <v>75.61476534182927</v>
+      </c>
+      <c r="E155" t="n">
+        <v>10</v>
+      </c>
+      <c r="F155" t="n">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6">
+      <c r="A156" t="s">
+        <v>313</v>
+      </c>
+      <c r="B156" t="n">
+        <v>0.7995296090894082</v>
+      </c>
+      <c r="C156" t="n">
+        <v>6.822892871604467e-08</v>
+      </c>
+      <c r="D156" t="n">
+        <v>64.23998980295708</v>
+      </c>
+      <c r="E156" t="n">
+        <v>10</v>
+      </c>
+      <c r="F156" t="n">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6">
+      <c r="A157" t="s">
+        <v>312</v>
+      </c>
+      <c r="B157" t="n">
+        <v>0.9958676758203767</v>
+      </c>
+      <c r="C157" t="n">
+        <v>6.633932736883973e-08</v>
+      </c>
+      <c r="D157" t="n">
+        <v>58.68636064613134</v>
+      </c>
+      <c r="E157" t="n">
+        <v>10</v>
+      </c>
+      <c r="F157" t="n">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6">
+      <c r="A158" t="s">
+        <v>313</v>
+      </c>
+      <c r="B158" t="n">
+        <v>0.9958676758203767</v>
+      </c>
+      <c r="C158" t="n">
+        <v>8.130486295054277e-08</v>
+      </c>
+      <c r="D158" t="n">
+        <v>54.42908682175597</v>
+      </c>
+      <c r="E158" t="n">
+        <v>10</v>
+      </c>
+      <c r="F158" t="n">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6">
+      <c r="A159" t="s">
+        <v>314</v>
+      </c>
+      <c r="B159" t="n">
+        <v>0.6031381429555186</v>
+      </c>
+      <c r="C159" t="n">
+        <v>2.107836171289383e-08</v>
+      </c>
+      <c r="D159" t="n">
+        <v>120.463001774684</v>
+      </c>
+      <c r="E159" t="n">
+        <v>10</v>
+      </c>
+      <c r="F159" t="n">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6">
+      <c r="A160" t="s">
+        <v>315</v>
+      </c>
+      <c r="B160" t="n">
+        <v>-1.208950593122265</v>
+      </c>
+      <c r="C160" t="n">
+        <v>9.589771445283666e-08</v>
+      </c>
+      <c r="D160" t="n">
+        <v>48.92815467636639</v>
+      </c>
+      <c r="E160" t="n">
+        <v>10</v>
+      </c>
+      <c r="F160" t="n">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6">
+      <c r="A161" t="s">
+        <v>314</v>
+      </c>
+      <c r="B161" t="n">
+        <v>1.008272875878131</v>
+      </c>
+      <c r="C161" t="n">
+        <v>6.679128859139235e-08</v>
+      </c>
+      <c r="D161" t="n">
+        <v>58.02225204973406</v>
+      </c>
+      <c r="E161" t="n">
+        <v>10</v>
+      </c>
+      <c r="F161" t="n">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6">
+      <c r="A162" t="s">
+        <v>315</v>
+      </c>
+      <c r="B162" t="n">
+        <v>-1.009770284191225</v>
+      </c>
+      <c r="C162" t="n">
+        <v>8.191297778073059e-08</v>
+      </c>
+      <c r="D162" t="n">
+        <v>53.95413155367921</v>
+      </c>
+      <c r="E162" t="n">
+        <v>10</v>
+      </c>
+      <c r="F162" t="n">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6">
+      <c r="A163" t="s">
+        <v>306</v>
+      </c>
+      <c r="B163" t="s">
+        <v>307</v>
+      </c>
+      <c r="C163" t="s">
+        <v>308</v>
+      </c>
+      <c r="D163" t="s">
+        <v>309</v>
+      </c>
+      <c r="E163" t="s">
+        <v>310</v>
+      </c>
+      <c r="F163" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6">
+      <c r="A164" t="s">
+        <v>312</v>
+      </c>
+      <c r="B164" t="n">
+        <v>0.9973294741275325</v>
+      </c>
+      <c r="C164" t="n">
+        <v>7.046664279168407e-08</v>
+      </c>
+      <c r="D164" t="n">
+        <v>46.9044173563351</v>
+      </c>
+      <c r="E164" t="n">
+        <v>10</v>
+      </c>
+      <c r="F164" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6">
+      <c r="A165" t="s">
+        <v>313</v>
+      </c>
+      <c r="B165" t="n">
+        <v>0.9973294741275325</v>
+      </c>
+      <c r="C165" t="n">
+        <v>7.792276057418851e-08</v>
+      </c>
+      <c r="D165" t="n">
+        <v>45.97836881123182</v>
+      </c>
+      <c r="E165" t="n">
+        <v>10</v>
+      </c>
+      <c r="F165" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6">
+      <c r="A166" t="s">
+        <v>312</v>
+      </c>
+      <c r="B166" t="n">
+        <v>0.9963977444986778</v>
+      </c>
+      <c r="C166" t="n">
+        <v>7.040083420451023e-08</v>
+      </c>
+      <c r="D166" t="n">
+        <v>46.92376456256169</v>
+      </c>
+      <c r="E166" t="n">
+        <v>10</v>
+      </c>
+      <c r="F166" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6">
+      <c r="A167" t="s">
+        <v>313</v>
+      </c>
+      <c r="B167" t="n">
+        <v>0.9963977444986778</v>
+      </c>
+      <c r="C167" t="n">
+        <v>7.785661623516875e-08</v>
+      </c>
+      <c r="D167" t="n">
+        <v>45.99391401214702</v>
+      </c>
+      <c r="E167" t="n">
+        <v>10</v>
+      </c>
+      <c r="F167" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6">
+      <c r="A168" t="s">
+        <v>314</v>
+      </c>
+      <c r="B168" t="n">
+        <v>0.9940380213056561</v>
+      </c>
+      <c r="C168" t="n">
+        <v>6.955107158972439e-08</v>
+      </c>
+      <c r="D168" t="n">
+        <v>46.97304965662369</v>
+      </c>
+      <c r="E168" t="n">
+        <v>10</v>
+      </c>
+      <c r="F168" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6">
+      <c r="A169" t="s">
+        <v>315</v>
+      </c>
+      <c r="B169" t="n">
+        <v>-0.9944052323547421</v>
+      </c>
+      <c r="C169" t="n">
+        <v>7.69877269031765e-08</v>
+      </c>
+      <c r="D169" t="n">
+        <v>46.02731190790848</v>
+      </c>
+      <c r="E169" t="n">
+        <v>10</v>
+      </c>
+      <c r="F169" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6">
+      <c r="A170" t="s">
+        <v>314</v>
+      </c>
+      <c r="B170" t="n">
+        <v>0.9995415393538161</v>
+      </c>
+      <c r="C170" t="n">
+        <v>7.025799300721906e-08</v>
+      </c>
+      <c r="D170" t="n">
+        <v>46.85873792392448</v>
+      </c>
+      <c r="E170" t="n">
+        <v>10</v>
+      </c>
+      <c r="F170" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6">
+      <c r="A171" t="s">
+        <v>315</v>
+      </c>
+      <c r="B171" t="n">
+        <v>-1.003509453937662</v>
+      </c>
+      <c r="C171" t="n">
+        <v>7.826618920119754e-08</v>
+      </c>
+      <c r="D171" t="n">
+        <v>45.87640989197381</v>
+      </c>
+      <c r="E171" t="n">
+        <v>10</v>
+      </c>
+      <c r="F171" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6">
+      <c r="A172" t="s">
+        <v>306</v>
+      </c>
+      <c r="B172" t="s">
+        <v>307</v>
+      </c>
+      <c r="C172" t="s">
+        <v>308</v>
+      </c>
+      <c r="D172" t="s">
+        <v>309</v>
+      </c>
+      <c r="E172" t="s">
+        <v>310</v>
+      </c>
+      <c r="F172" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6">
+      <c r="A173" t="s">
+        <v>312</v>
+      </c>
+      <c r="B173" t="n">
+        <v>1.006061220950502</v>
+      </c>
+      <c r="C173" t="n">
+        <v>7.108370226744208e-08</v>
+      </c>
+      <c r="D173" t="n">
+        <v>46.72615137605584</v>
+      </c>
+      <c r="E173" t="n">
+        <v>10</v>
+      </c>
+      <c r="F173" t="n">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6">
+      <c r="A174" t="s">
+        <v>313</v>
+      </c>
+      <c r="B174" t="n">
+        <v>1.006061220950502</v>
+      </c>
+      <c r="C174" t="n">
+        <v>7.854290768786771e-08</v>
+      </c>
+      <c r="D174" t="n">
+        <v>45.83488497347508</v>
+      </c>
+      <c r="E174" t="n">
+        <v>10</v>
+      </c>
+      <c r="F174" t="n">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6">
+      <c r="A175" t="s">
+        <v>312</v>
+      </c>
+      <c r="B175" t="n">
+        <v>0.9980367560893952</v>
+      </c>
+      <c r="C175" t="n">
+        <v>7.051660310208586e-08</v>
+      </c>
+      <c r="D175" t="n">
+        <v>46.88977316224476</v>
+      </c>
+      <c r="E175" t="n">
+        <v>10</v>
+      </c>
+      <c r="F175" t="n">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6">
+      <c r="A176" t="s">
+        <v>313</v>
+      </c>
+      <c r="B176" t="n">
+        <v>0.9980367560893952</v>
+      </c>
+      <c r="C176" t="n">
+        <v>7.797297493786842e-08</v>
+      </c>
+      <c r="D176" t="n">
+        <v>45.96659889941934</v>
+      </c>
+      <c r="E176" t="n">
+        <v>10</v>
+      </c>
+      <c r="F176" t="n">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6">
+      <c r="A177" t="s">
+        <v>314</v>
+      </c>
+      <c r="B177" t="n">
+        <v>0.985829282911027</v>
+      </c>
+      <c r="C177" t="n">
+        <v>6.908578084544552e-08</v>
+      </c>
+      <c r="D177" t="n">
+        <v>47.14774880993969</v>
+      </c>
+      <c r="E177" t="n">
+        <v>10</v>
+      </c>
+      <c r="F177" t="n">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6">
+      <c r="A178" t="s">
+        <v>315</v>
+      </c>
+      <c r="B178" t="n">
+        <v>-0.9890771184461969</v>
+      </c>
+      <c r="C178" t="n">
+        <v>7.695797514448837e-08</v>
+      </c>
+      <c r="D178" t="n">
+        <v>46.11766560563498</v>
+      </c>
+      <c r="E178" t="n">
+        <v>10</v>
+      </c>
+      <c r="F178" t="n">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6">
+      <c r="A179" t="s">
+        <v>314</v>
+      </c>
+      <c r="B179" t="n">
+        <v>0.992660621599613</v>
+      </c>
+      <c r="C179" t="n">
+        <v>6.94849977385302e-08</v>
+      </c>
+      <c r="D179" t="n">
+        <v>47.00200882673921</v>
+      </c>
+      <c r="E179" t="n">
+        <v>10</v>
+      </c>
+      <c r="F179" t="n">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6">
+      <c r="A180" t="s">
+        <v>315</v>
+      </c>
+      <c r="B180" t="n">
+        <v>-0.9981627842198529</v>
+      </c>
+      <c r="C180" t="n">
+        <v>7.76852735921519e-08</v>
+      </c>
+      <c r="D180" t="n">
+        <v>45.96450442024348</v>
+      </c>
+      <c r="E180" t="n">
+        <v>10</v>
+      </c>
+      <c r="F180" t="n">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6">
+      <c r="A181" t="s">
+        <v>306</v>
+      </c>
+      <c r="B181" t="s">
+        <v>307</v>
+      </c>
+      <c r="C181" t="s">
+        <v>308</v>
+      </c>
+      <c r="D181" t="s">
+        <v>309</v>
+      </c>
+      <c r="E181" t="s">
+        <v>310</v>
+      </c>
+      <c r="F181" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6">
+      <c r="A182" t="s">
+        <v>312</v>
+      </c>
+      <c r="B182" t="n">
+        <v>0.9966370632132333</v>
+      </c>
+      <c r="C182" t="n">
+        <v>1.408354735260481e-08</v>
+      </c>
+      <c r="D182" t="n">
+        <v>46.91878907694804</v>
+      </c>
+      <c r="E182" t="n">
+        <v>100</v>
+      </c>
+      <c r="F182" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6">
+      <c r="A183" t="s">
+        <v>313</v>
+      </c>
+      <c r="B183" t="n">
+        <v>0.9966370632132333</v>
+      </c>
+      <c r="C183" t="n">
+        <v>1.557472103002961e-08</v>
+      </c>
+      <c r="D183" t="n">
+        <v>45.98991678558544</v>
+      </c>
+      <c r="E183" t="n">
+        <v>100</v>
+      </c>
+      <c r="F183" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6">
+      <c r="A184" t="s">
+        <v>312</v>
+      </c>
+      <c r="B184" t="n">
+        <v>1.006366687377298</v>
+      </c>
+      <c r="C184" t="n">
+        <v>1.422105997075041e-08</v>
+      </c>
+      <c r="D184" t="n">
+        <v>46.72001316667031</v>
+      </c>
+      <c r="E184" t="n">
+        <v>100</v>
+      </c>
+      <c r="F184" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6">
+      <c r="A185" t="s">
+        <v>313</v>
+      </c>
+      <c r="B185" t="n">
+        <v>1.006366687377298</v>
+      </c>
+      <c r="C185" t="n">
+        <v>1.57129222782407e-08</v>
+      </c>
+      <c r="D185" t="n">
+        <v>45.82993634722494</v>
+      </c>
+      <c r="E185" t="n">
+        <v>100</v>
+      </c>
+      <c r="F185" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6">
+      <c r="A186" t="s">
+        <v>314</v>
+      </c>
+      <c r="B186" t="n">
+        <v>1.008627712022325</v>
+      </c>
+      <c r="C186" t="n">
+        <v>1.423272617339147e-08</v>
+      </c>
+      <c r="D186" t="n">
+        <v>46.67478158571797</v>
+      </c>
+      <c r="E186" t="n">
+        <v>100</v>
+      </c>
+      <c r="F186" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6">
+      <c r="A187" t="s">
+        <v>315</v>
+      </c>
+      <c r="B187" t="n">
+        <v>-1.004570811910261</v>
+      </c>
+      <c r="C187" t="n">
+        <v>1.560204150920829e-08</v>
+      </c>
+      <c r="D187" t="n">
+        <v>45.85909801515762</v>
+      </c>
+      <c r="E187" t="n">
+        <v>100</v>
+      </c>
+      <c r="F187" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6">
+      <c r="A188" t="s">
+        <v>314</v>
+      </c>
+      <c r="B188" t="n">
+        <v>0.9971289979726106</v>
+      </c>
+      <c r="C188" t="n">
+        <v>1.404530308330846e-08</v>
+      </c>
+      <c r="D188" t="n">
+        <v>46.90857484040909</v>
+      </c>
+      <c r="E188" t="n">
+        <v>100</v>
+      </c>
+      <c r="F188" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6">
+      <c r="A189" t="s">
+        <v>315</v>
+      </c>
+      <c r="B189" t="n">
+        <v>-0.9909466295467575</v>
+      </c>
+      <c r="C189" t="n">
+        <v>1.534849829907479e-08</v>
+      </c>
+      <c r="D189" t="n">
+        <v>46.08578794674555</v>
+      </c>
+      <c r="E189" t="n">
+        <v>100</v>
+      </c>
+      <c r="F189" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6">
+      <c r="A190" t="s">
+        <v>306</v>
+      </c>
+      <c r="B190" t="s">
+        <v>307</v>
+      </c>
+      <c r="C190" t="s">
+        <v>308</v>
+      </c>
+      <c r="D190" t="s">
+        <v>309</v>
+      </c>
+      <c r="E190" t="s">
+        <v>310</v>
+      </c>
+      <c r="F190" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6">
+      <c r="A191" t="s">
+        <v>312</v>
+      </c>
+      <c r="B191" t="n">
+        <v>0.9966370632132313</v>
+      </c>
+      <c r="C191" t="n">
+        <v>1.408354735260478e-08</v>
+      </c>
+      <c r="D191" t="n">
+        <v>46.91878907694808</v>
+      </c>
+      <c r="E191" t="n">
+        <v>100</v>
+      </c>
+      <c r="F191" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6">
+      <c r="A192" t="s">
+        <v>313</v>
+      </c>
+      <c r="B192" t="n">
+        <v>0.9966370632132313</v>
+      </c>
+      <c r="C192" t="n">
+        <v>1.557472103002958e-08</v>
+      </c>
+      <c r="D192" t="n">
+        <v>45.98991678558546</v>
+      </c>
+      <c r="E192" t="n">
+        <v>100</v>
+      </c>
+      <c r="F192" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6">
+      <c r="A193" t="s">
+        <v>312</v>
+      </c>
+      <c r="B193" t="n">
+        <v>1.006366687377301</v>
+      </c>
+      <c r="C193" t="n">
+        <v>1.422105997075044e-08</v>
+      </c>
+      <c r="D193" t="n">
+        <v>46.72001316667027</v>
+      </c>
+      <c r="E193" t="n">
+        <v>100</v>
+      </c>
+      <c r="F193" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6">
+      <c r="A194" t="s">
+        <v>313</v>
+      </c>
+      <c r="B194" t="n">
+        <v>1.006366687377301</v>
+      </c>
+      <c r="C194" t="n">
+        <v>1.571292227824073e-08</v>
+      </c>
+      <c r="D194" t="n">
+        <v>45.82993634722488</v>
+      </c>
+      <c r="E194" t="n">
+        <v>100</v>
+      </c>
+      <c r="F194" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6">
+      <c r="A195" t="s">
+        <v>314</v>
+      </c>
+      <c r="B195" t="n">
+        <v>1.008627712022326</v>
+      </c>
+      <c r="C195" t="n">
+        <v>1.423272617339148e-08</v>
+      </c>
+      <c r="D195" t="n">
+        <v>46.67478158571795</v>
+      </c>
+      <c r="E195" t="n">
+        <v>100</v>
+      </c>
+      <c r="F195" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6">
+      <c r="A196" t="s">
+        <v>315</v>
+      </c>
+      <c r="B196" t="n">
+        <v>-1.004570811910262</v>
+      </c>
+      <c r="C196" t="n">
+        <v>1.56020415092083e-08</v>
+      </c>
+      <c r="D196" t="n">
+        <v>45.85909801515762</v>
+      </c>
+      <c r="E196" t="n">
+        <v>100</v>
+      </c>
+      <c r="F196" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6">
+      <c r="A197" t="s">
+        <v>314</v>
+      </c>
+      <c r="B197" t="n">
+        <v>0.9971289979726076</v>
+      </c>
+      <c r="C197" t="n">
+        <v>1.404530308330841e-08</v>
+      </c>
+      <c r="D197" t="n">
+        <v>46.90857484040914</v>
+      </c>
+      <c r="E197" t="n">
+        <v>100</v>
+      </c>
+      <c r="F197" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6">
+      <c r="A198" t="s">
+        <v>315</v>
+      </c>
+      <c r="B198" t="n">
+        <v>-0.985262925717436</v>
+      </c>
+      <c r="C198" t="n">
+        <v>1.518104744304541e-08</v>
+      </c>
+      <c r="D198" t="n">
+        <v>46.18329593821608</v>
+      </c>
+      <c r="E198" t="n">
+        <v>100</v>
+      </c>
+      <c r="F198" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6">
+      <c r="A199" t="s">
+        <v>306</v>
+      </c>
+      <c r="B199" t="s">
+        <v>307</v>
+      </c>
+      <c r="C199" t="s">
+        <v>308</v>
+      </c>
+      <c r="D199" t="s">
+        <v>309</v>
+      </c>
+      <c r="E199" t="s">
+        <v>310</v>
+      </c>
+      <c r="F199" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6">
+      <c r="A200" t="s">
+        <v>312</v>
+      </c>
+      <c r="B200" t="n">
+        <v>0.9875831140021362</v>
+      </c>
+      <c r="C200" t="n">
+        <v>6.977859551384201e-09</v>
+      </c>
+      <c r="D200" t="n">
+        <v>47.10999329659687</v>
+      </c>
+      <c r="E200" t="n">
+        <v>100</v>
+      </c>
+      <c r="F200" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6">
+      <c r="A201" t="s">
+        <v>313</v>
+      </c>
+      <c r="B201" t="n">
+        <v>0.9875831140021362</v>
+      </c>
+      <c r="C201" t="n">
+        <v>7.723113962096876e-09</v>
+      </c>
+      <c r="D201" t="n">
+        <v>46.14327743455643</v>
+      </c>
+      <c r="E201" t="n">
+        <v>100</v>
+      </c>
+      <c r="F201" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6">
+      <c r="A202" t="s">
+        <v>312</v>
+      </c>
+      <c r="B202" t="n">
+        <v>0.9951580830885313</v>
+      </c>
+      <c r="C202" t="n">
+        <v>7.031328690698309e-09</v>
+      </c>
+      <c r="D202" t="n">
+        <v>46.94960480983654</v>
+      </c>
+      <c r="E202" t="n">
+        <v>100</v>
+      </c>
+      <c r="F202" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6">
+      <c r="A203" t="s">
+        <v>313</v>
+      </c>
+      <c r="B203" t="n">
+        <v>0.9951580830885313</v>
+      </c>
+      <c r="C203" t="n">
+        <v>7.776862031408812e-09</v>
+      </c>
+      <c r="D203" t="n">
+        <v>46.0146680493738</v>
+      </c>
+      <c r="E203" t="n">
+        <v>100</v>
+      </c>
+      <c r="F203" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6">
+      <c r="A204" t="s">
+        <v>314</v>
+      </c>
+      <c r="B204" t="n">
+        <v>1.011209481021073</v>
+      </c>
+      <c r="C204" t="n">
+        <v>7.091106651001583e-09</v>
+      </c>
+      <c r="D204" t="n">
+        <v>46.6235667640778</v>
+      </c>
+      <c r="E204" t="n">
+        <v>100</v>
+      </c>
+      <c r="F204" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6">
+      <c r="A205" t="s">
+        <v>315</v>
+      </c>
+      <c r="B205" t="n">
+        <v>-1.015823453798906</v>
+      </c>
+      <c r="C205" t="n">
+        <v>7.900039772079465e-09</v>
+      </c>
+      <c r="D205" t="n">
+        <v>45.67904590911876</v>
+      </c>
+      <c r="E205" t="n">
+        <v>100</v>
+      </c>
+      <c r="F205" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6">
+      <c r="A206" t="s">
+        <v>314</v>
+      </c>
+      <c r="B206" t="n">
+        <v>1.002951284556005</v>
+      </c>
+      <c r="C206" t="n">
+        <v>7.027965099202063e-09</v>
+      </c>
+      <c r="D206" t="n">
+        <v>46.78901843913067</v>
+      </c>
+      <c r="E206" t="n">
+        <v>100</v>
+      </c>
+      <c r="F206" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6">
+      <c r="A207" t="s">
+        <v>315</v>
+      </c>
+      <c r="B207" t="n">
+        <v>-1.008902719070079</v>
+      </c>
+      <c r="C207" t="n">
+        <v>7.855905534717244e-09</v>
+      </c>
+      <c r="D207" t="n">
+        <v>45.78903421397283</v>
+      </c>
+      <c r="E207" t="n">
+        <v>100</v>
+      </c>
+      <c r="F207" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6">
+      <c r="A208" t="s">
+        <v>306</v>
+      </c>
+      <c r="B208" t="s">
+        <v>307</v>
+      </c>
+      <c r="C208" t="s">
+        <v>308</v>
+      </c>
+      <c r="D208" t="s">
+        <v>309</v>
+      </c>
+      <c r="E208" t="s">
+        <v>310</v>
+      </c>
+      <c r="F208" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6">
+      <c r="A209" t="s">
+        <v>312</v>
+      </c>
+      <c r="B209" t="n">
+        <v>0.9966593864362249</v>
+      </c>
+      <c r="C209" t="n">
+        <v>7.041931342670945e-09</v>
+      </c>
+      <c r="D209" t="n">
+        <v>46.91832518682047</v>
+      </c>
+      <c r="E209" t="n">
+        <v>100</v>
+      </c>
+      <c r="F209" t="n">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6">
+      <c r="A210" t="s">
+        <v>313</v>
+      </c>
+      <c r="B210" t="n">
+        <v>0.9966593864362249</v>
+      </c>
+      <c r="C210" t="n">
+        <v>7.787518986487651e-09</v>
+      </c>
+      <c r="D210" t="n">
+        <v>45.98954408579414</v>
+      </c>
+      <c r="E210" t="n">
+        <v>100</v>
+      </c>
+      <c r="F210" t="n">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6">
+      <c r="A211" t="s">
+        <v>312</v>
+      </c>
+      <c r="B211" t="n">
+        <v>0.986371946407253</v>
+      </c>
+      <c r="C211" t="n">
+        <v>6.969314638681144e-09</v>
+      </c>
+      <c r="D211" t="n">
+        <v>47.13604135857159</v>
+      </c>
+      <c r="E211" t="n">
+        <v>100</v>
+      </c>
+      <c r="F211" t="n">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6">
+      <c r="A212" t="s">
+        <v>313</v>
+      </c>
+      <c r="B212" t="n">
+        <v>-417.1281806923286</v>
+      </c>
+      <c r="C212" t="n">
+        <v>0.00131377796910028</v>
+      </c>
+      <c r="D212" t="n">
+        <v>38.00004367919664</v>
+      </c>
+      <c r="E212" t="n">
+        <v>100</v>
+      </c>
+      <c r="F212" t="n">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6">
+      <c r="A213" t="s">
+        <v>314</v>
+      </c>
+      <c r="B213" t="n">
+        <v>1.011667285328351</v>
+      </c>
+      <c r="C213" t="n">
+        <v>7.140557129528449e-09</v>
+      </c>
+      <c r="D213" t="n">
+        <v>46.61453307147693</v>
+      </c>
+      <c r="E213" t="n">
+        <v>100</v>
+      </c>
+      <c r="F213" t="n">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6">
+      <c r="A214" t="s">
+        <v>315</v>
+      </c>
+      <c r="B214" t="n">
+        <v>-1.010335295815346</v>
+      </c>
+      <c r="C214" t="n">
+        <v>7.866063201847132e-09</v>
+      </c>
+      <c r="D214" t="n">
+        <v>45.76607190502735</v>
+      </c>
+      <c r="E214" t="n">
+        <v>100</v>
+      </c>
+      <c r="F214" t="n">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6">
+      <c r="A215" t="s">
+        <v>314</v>
+      </c>
+      <c r="B215" t="n">
+        <v>1.018956402441949</v>
+      </c>
+      <c r="C215" t="n">
+        <v>7.171064776703011e-09</v>
+      </c>
+      <c r="D215" t="n">
+        <v>46.47260921388353</v>
+      </c>
+      <c r="E215" t="n">
+        <v>100</v>
+      </c>
+      <c r="F215" t="n">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6">
+      <c r="A216" t="s">
+        <v>315</v>
+      </c>
+      <c r="B216" t="n">
+        <v>1.020598466796085</v>
+      </c>
+      <c r="C216" t="n">
+        <v>7.938871371853881e-09</v>
+      </c>
+      <c r="D216" t="n">
+        <v>45.604524013785</v>
+      </c>
+      <c r="E216" t="n">
+        <v>100</v>
+      </c>
+      <c r="F216" t="n">
+        <v>-100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
 </file>
</xml_diff>